<commit_message>
feat: change stylings on radio buttons
</commit_message>
<xml_diff>
--- a/CSM.xlsx
+++ b/CSM.xlsx
@@ -1,26 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27328"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xml:space="preserve">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr codeName="ThisWorkbook"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jaypee\Desktop\My Stuff\CSM\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C72FD34B-365C-45CC-8B3E-0AC8E3B8F7DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView activeTab="0" autoFilterDateGrouping="true" firstSheet="0" minimized="false" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="600" visibility="visible"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <definedNames/>
+  <calcPr calcId="999999" calcMode="auto" calcCompleted="1" fullCalcOnLoad="0" forceFullCalc="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="54">
   <si>
     <t>Demographic</t>
   </si>
@@ -176,42 +171,66 @@
   </si>
   <si>
     <t>Somewhat helped.</t>
+  </si>
+  <si>
+    <t>ASDS</t>
+  </si>
+  <si>
+    <t>Other request or inqueries</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xml:space="preserve">
+  <numFmts count="0"/>
+  <fonts count="5">
     <font>
+      <b val="0"/>
+      <i val="0"/>
+      <strike val="0"/>
+      <u val="none"/>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
+      <b val="1"/>
+      <i val="0"/>
+      <strike val="0"/>
+      <u val="none"/>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
+      <b val="1"/>
+      <i val="0"/>
+      <strike val="0"/>
+      <u val="none"/>
       <sz val="9"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="18"/>
+      <b val="0"/>
+      <i val="0"/>
+      <strike val="0"/>
+      <u val="none"/>
+      <sz val="9"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="9"/>
+      <b val="1"/>
+      <i val="0"/>
+      <strike val="0"/>
+      <u val="none"/>
+      <sz val="18"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <scheme val="minor"/>
@@ -326,51 +345,43 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="11">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="0" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0"/>
+    <xf xfId="0" fontId="1" numFmtId="0" fillId="2" borderId="1" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" shrinkToFit="false"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf xfId="0" fontId="2" numFmtId="0" fillId="3" borderId="1" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" shrinkToFit="false"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf xfId="0" fontId="2" numFmtId="0" fillId="4" borderId="1" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" shrinkToFit="false"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="1" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" shrinkToFit="false"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf xfId="0" fontId="3" numFmtId="0" fillId="0" borderId="1" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" shrinkToFit="false"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf xfId="0" fontId="4" numFmtId="0" fillId="5" borderId="2" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf xfId="0" fontId="4" numFmtId="0" fillId="5" borderId="3" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf xfId="0" fontId="4" numFmtId="0" fillId="5" borderId="4" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf xfId="0" fontId="4" numFmtId="0" fillId="6" borderId="1" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf xfId="0" fontId="4" numFmtId="0" fillId="7" borderId="1" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <tableStyles defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotTableStyle1"/>
 </styleSheet>
 </file>
 
@@ -694,23 +705,39 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:R12"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xml:space="preserve" mc:Ignorable="x14ac">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+  </sheetPr>
+  <dimension ref="A1:R13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="P1" zoomScale="96" zoomScaleNormal="96" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0" zoomScale="96" zoomScaleNormal="96" showGridLines="true" showRowColHeaders="1" topLeftCell="P1">
       <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="6" width="20.7109375" customWidth="1"/>
-    <col min="7" max="7" width="37.140625" customWidth="1"/>
-    <col min="8" max="8" width="29.42578125" customWidth="1"/>
-    <col min="9" max="9" width="20.85546875" customWidth="1"/>
-    <col min="10" max="18" width="40.7109375" customWidth="1"/>
+    <col min="1" max="1" width="20.7109375" customWidth="true" style="0"/>
+    <col min="2" max="2" width="20.7109375" customWidth="true" style="0"/>
+    <col min="3" max="3" width="20.7109375" customWidth="true" style="0"/>
+    <col min="4" max="4" width="20.7109375" customWidth="true" style="0"/>
+    <col min="5" max="5" width="20.7109375" customWidth="true" style="0"/>
+    <col min="6" max="6" width="20.7109375" customWidth="true" style="0"/>
+    <col min="7" max="7" width="37.140625" customWidth="true" style="0"/>
+    <col min="8" max="8" width="29.42578125" customWidth="true" style="0"/>
+    <col min="9" max="9" width="20.85546875" customWidth="true" style="0"/>
+    <col min="10" max="10" width="40.7109375" customWidth="true" style="0"/>
+    <col min="11" max="11" width="40.7109375" customWidth="true" style="0"/>
+    <col min="12" max="12" width="40.7109375" customWidth="true" style="0"/>
+    <col min="13" max="13" width="40.7109375" customWidth="true" style="0"/>
+    <col min="14" max="14" width="40.7109375" customWidth="true" style="0"/>
+    <col min="15" max="15" width="40.7109375" customWidth="true" style="0"/>
+    <col min="16" max="16" width="40.7109375" customWidth="true" style="0"/>
+    <col min="17" max="17" width="40.7109375" customWidth="true" style="0"/>
+    <col min="18" max="18" width="40.7109375" customWidth="true" style="0"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:18" customHeight="1" ht="51.75">
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
@@ -736,7 +763,7 @@
       <c r="Q1" s="10"/>
       <c r="R1" s="10"/>
     </row>
-    <row r="2" spans="1:18" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:18" customHeight="1" ht="39.95">
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
@@ -792,7 +819,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:18" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:18" customHeight="1" ht="39.95">
       <c r="A3" s="4" t="s">
         <v>21</v>
       </c>
@@ -848,7 +875,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="4" spans="1:18" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:18" customHeight="1" ht="39.95">
       <c r="A4" s="4" t="s">
         <v>29</v>
       </c>
@@ -904,7 +931,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="5" spans="1:18" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:18" customHeight="1" ht="39.95">
       <c r="A5" s="4" t="s">
         <v>29</v>
       </c>
@@ -960,7 +987,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="6" spans="1:18" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:18" customHeight="1" ht="39.95">
       <c r="A6" s="4" t="s">
         <v>21</v>
       </c>
@@ -1016,7 +1043,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="7" spans="1:18" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:18" customHeight="1" ht="39.95">
       <c r="A7" s="4" t="s">
         <v>29</v>
       </c>
@@ -1072,7 +1099,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="8" spans="1:18" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:18" customHeight="1" ht="39.95">
       <c r="A8" s="4" t="s">
         <v>29</v>
       </c>
@@ -1128,7 +1155,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="9" spans="1:18" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:18" customHeight="1" ht="39.95">
       <c r="A9" s="4" t="s">
         <v>46</v>
       </c>
@@ -1184,7 +1211,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="10" spans="1:18" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:18" customHeight="1" ht="39.95">
       <c r="A10" s="4" t="s">
         <v>46</v>
       </c>
@@ -1240,7 +1267,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="11" spans="1:18" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:18" customHeight="1" ht="39.95">
       <c r="A11" s="4" t="s">
         <v>21</v>
       </c>
@@ -1296,7 +1323,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="12" spans="1:18" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:18" customHeight="1" ht="39.95">
       <c r="A12" s="4" t="s">
         <v>29</v>
       </c>
@@ -1352,13 +1379,70 @@
         <v>33</v>
       </c>
     </row>
+    <row r="13" spans="1:18" customHeight="1" ht="39.95">
+      <c r="A13" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="C13" s="4">
+        <v>89</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="E13" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="F13" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="G13" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="H13" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="I13" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="J13" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="K13" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="L13" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="M13" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="N13" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="O13" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="P13" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q13" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="R13" s="5" t="s">
+        <v>33</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells>
     <mergeCell ref="A1:F1"/>
     <mergeCell ref="G1:I1"/>
     <mergeCell ref="J1:R1"/>
   </mergeCells>
+  <printOptions gridLines="false" gridLinesSet="true"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" scale="100" fitToHeight="1" fitToWidth="1" pageOrder="downThenOver" r:id="rId1ps"/>
 </worksheet>
 </file>
</xml_diff>